<commit_message>
changes in wraper method to show only one match for each question
</commit_message>
<xml_diff>
--- a/src/resources/factes_by_org/facets149.xlsx
+++ b/src/resources/factes_by_org/facets149.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">What is your CTC?</t>
   </si>
   <si>
-    <t xml:space="preserve">Are you his/her father?</t>
+    <t xml:space="preserve">Are you child’s father?</t>
   </si>
   <si>
     <t xml:space="preserve">What is his per centage?</t>
@@ -95,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -130,11 +130,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,7 +174,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,10 +188,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -220,7 +211,7 @@
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -300,7 +291,7 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -402,11 +393,11 @@
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2"/>
@@ -431,7 +422,7 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3"/>

</xml_diff>